<commit_message>
changed code to fetch data from excel sheet using row name and column name. Also using data provider to test valid and invalid code in text editor in a single @Test method(stack module)
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\git\Testng_Ninjalinos\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9419EBC8-6F9D-4B1C-876F-A97037E1D2F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4CD756-268F-4671-8045-C0DA88534252}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,7 +194,7 @@
     <t>validcode</t>
   </si>
   <si>
-    <t>invlaidcode</t>
+    <t>invalidcode</t>
   </si>
 </sst>
 </file>
@@ -639,7 +639,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>